<commit_message>
1.remove object type 2.improve code robustness
</commit_message>
<xml_diff>
--- a/testcase/Exclude.xlsx
+++ b/testcase/Exclude.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BDD7F2B6-6129-4971-9C53-2F03837C62AC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FCD391-91E6-4E9A-9F9D-F0258B515E2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude" sheetId="1" r:id="rId1"/>
@@ -15,17 +15,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>Exclude Table</t>
-  </si>
-  <si>
-    <t>Exclude</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -45,6 +39,9 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>#Exclude Table</t>
   </si>
 </sst>
 </file>
@@ -442,17 +439,14 @@
   <dimension ref="L1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="12:13">
       <c r="L1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="12:13">
@@ -460,15 +454,15 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="12:13">
       <c r="L3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="12:13">
@@ -476,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="12:13">
@@ -484,7 +478,7 @@
         <v>2</v>
       </c>
       <c r="M5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="12:13">
@@ -492,7 +486,7 @@
         <v>3</v>
       </c>
       <c r="M6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="12:13">
@@ -500,7 +494,7 @@
         <v>4</v>
       </c>
       <c r="M7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="12:13">
@@ -508,7 +502,7 @@
         <v>5</v>
       </c>
       <c r="M8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="12:13">

</xml_diff>